<commit_message>
fixed more extra commas in station names
</commit_message>
<xml_diff>
--- a/config/CERA_NOAA_HSOFS_stations_V3.xlsx
+++ b/config/CERA_NOAA_HSOFS_stations_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bblanton/GitHub/RENCI/ADCIRCSupportTools/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA96CEFE-E45A-2145-BD6C-BCE09189EFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7049351E-A8EA-B347-B9F9-E029B0906B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="700" windowWidth="33200" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,9 +480,6 @@
     <t>Dock E Port of Pascagoula</t>
   </si>
   <si>
-    <t>Pascagoula NOAA Lab</t>
-  </si>
-  <si>
     <t>Bay Waveland Yacht Club</t>
   </si>
   <si>
@@ -649,6 +646,9 @@
   </si>
   <si>
     <t>Texas Point/Sabine Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1390,7 +1390,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="79" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F1" s="79" t="s">
         <v>4</v>
@@ -1500,10 +1500,10 @@
         <v>32.373388890000001</v>
       </c>
       <c r="I3" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J3" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K3" s="85" t="s">
         <v>60</v>
@@ -2369,7 +2369,7 @@
         <v>8465705</v>
       </c>
       <c r="C20" s="83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D20" s="83" t="s">
         <v>48</v>
@@ -2647,10 +2647,10 @@
         <v>42.0139</v>
       </c>
       <c r="I25" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J25" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K25" s="85" t="s">
         <v>60</v>
@@ -6078,10 +6078,10 @@
         <v>30.416889999999999</v>
       </c>
       <c r="I91" s="76" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J91" s="76" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K91" s="88" t="s">
         <v>60</v>
@@ -6626,7 +6626,7 @@
         <v>8741533</v>
       </c>
       <c r="C102" s="83" t="s">
-        <v>146</v>
+        <v>202</v>
       </c>
       <c r="D102" s="83" t="s">
         <v>144</v>
@@ -6678,7 +6678,7 @@
         <v>8747437</v>
       </c>
       <c r="C103" s="83" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D103" s="83" t="s">
         <v>144</v>
@@ -6730,10 +6730,10 @@
         <v>8760721</v>
       </c>
       <c r="C104" s="83" t="s">
+        <v>147</v>
+      </c>
+      <c r="D104" s="83" t="s">
         <v>148</v>
-      </c>
-      <c r="D104" s="83" t="s">
-        <v>149</v>
       </c>
       <c r="E104" s="83" t="s">
         <v>21</v>
@@ -6755,7 +6755,7 @@
         <v>-0.23663517220359645</v>
       </c>
       <c r="K104" s="89" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L104" s="71">
         <v>-89.258309999999994</v>
@@ -6782,10 +6782,10 @@
         <v>8760922</v>
       </c>
       <c r="C105" s="83" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D105" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E105" s="83" t="s">
         <v>21</v>
@@ -6834,10 +6834,10 @@
         <v>8761305</v>
       </c>
       <c r="C106" s="83" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D106" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E106" s="83" t="s">
         <v>21</v>
@@ -6886,10 +6886,10 @@
         <v>8761724</v>
       </c>
       <c r="C107" s="83" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D107" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E107" s="83" t="s">
         <v>21</v>
@@ -6911,7 +6911,7 @@
         <v>-5.5531850045717764E-2</v>
       </c>
       <c r="K107" s="90" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L107" s="69">
         <v>-89.948939999999993</v>
@@ -6938,10 +6938,10 @@
         <v>8761927</v>
       </c>
       <c r="C108" s="83" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D108" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E108" s="83" t="s">
         <v>21</v>
@@ -6990,10 +6990,10 @@
         <v>8761955</v>
       </c>
       <c r="C109" s="83" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D109" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E109" s="83" t="s">
         <v>21</v>
@@ -7008,10 +7008,10 @@
         <v>29.93289</v>
       </c>
       <c r="I109" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J109" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K109" s="85" t="s">
         <v>60</v>
@@ -7041,10 +7041,10 @@
         <v>8762075</v>
       </c>
       <c r="C110" s="83" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D110" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E110" s="83" t="s">
         <v>21</v>
@@ -7059,10 +7059,10 @@
         <v>29.1142</v>
       </c>
       <c r="I110" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J110" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K110" s="85" t="s">
         <v>60</v>
@@ -7092,10 +7092,10 @@
         <v>8762482</v>
       </c>
       <c r="C111" s="83" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D111" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E111" s="83" t="s">
         <v>21</v>
@@ -7144,10 +7144,10 @@
         <v>8762483</v>
       </c>
       <c r="C112" s="83" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D112" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E112" s="83" t="s">
         <v>21</v>
@@ -7196,10 +7196,10 @@
         <v>8764044</v>
       </c>
       <c r="C113" s="83" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D113" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E113" s="83" t="s">
         <v>21</v>
@@ -7248,10 +7248,10 @@
         <v>8764227</v>
       </c>
       <c r="C114" s="83" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D114" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E114" s="83" t="s">
         <v>21</v>
@@ -7300,10 +7300,10 @@
         <v>8764314</v>
       </c>
       <c r="C115" s="83" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D115" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E115" s="83" t="s">
         <v>21</v>
@@ -7325,7 +7325,7 @@
         <v>-0.10953977445900639</v>
       </c>
       <c r="K115" s="89" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L115" s="71">
         <v>-91.383899999999997</v>
@@ -7352,10 +7352,10 @@
         <v>8766072</v>
       </c>
       <c r="C116" s="83" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D116" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E116" s="83" t="s">
         <v>21</v>
@@ -7370,13 +7370,13 @@
         <v>29.555</v>
       </c>
       <c r="I116" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="J116" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="K116" s="89" t="s">
         <v>190</v>
-      </c>
-      <c r="J116" s="70" t="s">
-        <v>190</v>
-      </c>
-      <c r="K116" s="89" t="s">
-        <v>191</v>
       </c>
       <c r="L116" s="71">
         <v>-92.305000000000007</v>
@@ -7403,10 +7403,10 @@
         <v>8767816</v>
       </c>
       <c r="C117" s="83" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D117" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E117" s="83" t="s">
         <v>21</v>
@@ -7455,10 +7455,10 @@
         <v>8767961</v>
       </c>
       <c r="C118" s="83" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D118" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E118" s="83" t="s">
         <v>21</v>
@@ -7507,10 +7507,10 @@
         <v>8768094</v>
       </c>
       <c r="C119" s="83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D119" s="83" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E119" s="83" t="s">
         <v>21</v>
@@ -7559,10 +7559,10 @@
         <v>8770570</v>
       </c>
       <c r="C120" s="83" t="s">
+        <v>164</v>
+      </c>
+      <c r="D120" s="83" t="s">
         <v>165</v>
-      </c>
-      <c r="D120" s="83" t="s">
-        <v>166</v>
       </c>
       <c r="E120" s="83" t="s">
         <v>21</v>
@@ -7611,10 +7611,10 @@
         <v>8770613</v>
       </c>
       <c r="C121" s="83" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D121" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E121" s="83" t="s">
         <v>21</v>
@@ -7663,10 +7663,10 @@
         <v>8770822</v>
       </c>
       <c r="C122" s="83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D122" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E122" s="83" t="s">
         <v>21</v>
@@ -7681,13 +7681,13 @@
         <v>29.688330000000001</v>
       </c>
       <c r="I122" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="J122" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="K122" s="90" t="s">
         <v>190</v>
-      </c>
-      <c r="J122" s="70" t="s">
-        <v>190</v>
-      </c>
-      <c r="K122" s="90" t="s">
-        <v>191</v>
       </c>
       <c r="L122" s="69">
         <v>-93.839780000000005</v>
@@ -7714,10 +7714,10 @@
         <v>8771013</v>
       </c>
       <c r="C123" s="83" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D123" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E123" s="83" t="s">
         <v>21</v>
@@ -7766,10 +7766,10 @@
         <v>8771450</v>
       </c>
       <c r="C124" s="83" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D124" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E124" s="83" t="s">
         <v>21</v>
@@ -7818,10 +7818,10 @@
         <v>8772447</v>
       </c>
       <c r="C125" s="83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D125" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E125" s="83" t="s">
         <v>21</v>
@@ -7870,10 +7870,10 @@
         <v>8772471</v>
       </c>
       <c r="C126" s="83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D126" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E126" s="83" t="s">
         <v>21</v>
@@ -7888,13 +7888,13 @@
         <v>28.934999999999999</v>
       </c>
       <c r="I126" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="J126" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="K126" s="89" t="s">
         <v>190</v>
-      </c>
-      <c r="J126" s="70" t="s">
-        <v>190</v>
-      </c>
-      <c r="K126" s="89" t="s">
-        <v>191</v>
       </c>
       <c r="L126" s="71">
         <v>-95.295000000000002</v>
@@ -7921,10 +7921,10 @@
         <v>8773767</v>
       </c>
       <c r="C127" s="83" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D127" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E127" s="83" t="s">
         <v>21</v>
@@ -7946,7 +7946,7 @@
         <v>-8.9911612313319095E-2</v>
       </c>
       <c r="K127" s="89" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L127" s="71">
         <v>-96.330100000000002</v>
@@ -7973,10 +7973,10 @@
         <v>8774770</v>
       </c>
       <c r="C128" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D128" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E128" s="83" t="s">
         <v>21</v>
@@ -8025,10 +8025,10 @@
         <v>8775241</v>
       </c>
       <c r="C129" s="83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D129" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E129" s="83" t="s">
         <v>21</v>
@@ -8043,13 +8043,13 @@
         <v>27.836670000000002</v>
       </c>
       <c r="I129" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="J129" s="70" t="s">
+        <v>189</v>
+      </c>
+      <c r="K129" s="89" t="s">
         <v>190</v>
-      </c>
-      <c r="J129" s="70" t="s">
-        <v>190</v>
-      </c>
-      <c r="K129" s="89" t="s">
-        <v>191</v>
       </c>
       <c r="L129" s="71">
         <v>-97.038330000000002</v>
@@ -8076,10 +8076,10 @@
         <v>8775870</v>
       </c>
       <c r="C130" s="83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D130" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E130" s="83" t="s">
         <v>21</v>
@@ -8128,10 +8128,10 @@
         <v>8779748</v>
       </c>
       <c r="C131" s="83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D131" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E131" s="83" t="s">
         <v>21</v>
@@ -8180,10 +8180,10 @@
         <v>8779770</v>
       </c>
       <c r="C132" s="83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D132" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E132" s="83" t="s">
         <v>21</v>
@@ -8232,10 +8232,10 @@
         <v>9751364</v>
       </c>
       <c r="C133" s="83" t="s">
+        <v>174</v>
+      </c>
+      <c r="D133" s="83" t="s">
         <v>175</v>
-      </c>
-      <c r="D133" s="83" t="s">
-        <v>176</v>
       </c>
       <c r="E133" s="83" t="s">
         <v>21</v>
@@ -8284,10 +8284,10 @@
         <v>9751381</v>
       </c>
       <c r="C134" s="83" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D134" s="83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E134" s="83" t="s">
         <v>21</v>
@@ -8336,10 +8336,10 @@
         <v>9751401</v>
       </c>
       <c r="C135" s="83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D135" s="83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E135" s="83" t="s">
         <v>21</v>
@@ -8388,10 +8388,10 @@
         <v>9751639</v>
       </c>
       <c r="C136" s="83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D136" s="83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E136" s="83" t="s">
         <v>21</v>
@@ -8440,10 +8440,10 @@
         <v>9752235</v>
       </c>
       <c r="C137" s="83" t="s">
+        <v>179</v>
+      </c>
+      <c r="D137" s="83" t="s">
         <v>180</v>
-      </c>
-      <c r="D137" s="83" t="s">
-        <v>181</v>
       </c>
       <c r="E137" s="83" t="s">
         <v>21</v>
@@ -8492,10 +8492,10 @@
         <v>9752695</v>
       </c>
       <c r="C138" s="83" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D138" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E138" s="83" t="s">
         <v>21</v>
@@ -8544,10 +8544,10 @@
         <v>9755371</v>
       </c>
       <c r="C139" s="83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D139" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E139" s="83" t="s">
         <v>21</v>
@@ -8596,10 +8596,10 @@
         <v>9759110</v>
       </c>
       <c r="C140" s="83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D140" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E140" s="83" t="s">
         <v>21</v>
@@ -8648,10 +8648,10 @@
         <v>9759394</v>
       </c>
       <c r="C141" s="83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D141" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E141" s="83" t="s">
         <v>21</v>
@@ -8700,10 +8700,10 @@
         <v>9759938</v>
       </c>
       <c r="C142" s="83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D142" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E142" s="83" t="s">
         <v>21</v>
@@ -8752,10 +8752,10 @@
         <v>9761115</v>
       </c>
       <c r="C143" s="83" t="s">
+        <v>186</v>
+      </c>
+      <c r="D143" s="83" t="s">
         <v>187</v>
-      </c>
-      <c r="D143" s="83" t="s">
-        <v>188</v>
       </c>
       <c r="E143" s="83" t="s">
         <v>21</v>
@@ -8770,10 +8770,10 @@
         <v>17.590689999999999</v>
       </c>
       <c r="I143" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J143" s="70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K143" s="85" t="s">
         <v>60</v>
@@ -13452,7 +13452,7 @@
         <v>8747437</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D42" s="32" t="s">
         <v>144</v>
@@ -13505,10 +13505,10 @@
         <v>8760721</v>
       </c>
       <c r="C43" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" s="44" t="s">
         <v>148</v>
-      </c>
-      <c r="D43" s="44" t="s">
-        <v>149</v>
       </c>
       <c r="E43" s="44" t="s">
         <v>22</v>
@@ -13527,7 +13527,7 @@
         <v>-0.23663517220359645</v>
       </c>
       <c r="J43" s="53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K43" s="37">
         <v>-89.258309999999994</v>
@@ -13558,10 +13558,10 @@
         <v>8761305</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E44" s="32" t="s">
         <v>22</v>
@@ -13611,10 +13611,10 @@
         <v>8761724</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E45" s="32" t="s">
         <v>22</v>
@@ -13633,7 +13633,7 @@
         <v>-5.5531850045717764E-2</v>
       </c>
       <c r="J45" s="54" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K45" s="48">
         <v>-89.948939999999993</v>
@@ -13664,10 +13664,10 @@
         <v>8764314</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E46" s="32" t="s">
         <v>22</v>
@@ -13686,7 +13686,7 @@
         <v>-0.10953977445900639</v>
       </c>
       <c r="J46" s="53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K46" s="37">
         <v>-91.383899999999997</v>
@@ -13717,10 +13717,10 @@
         <v>8766072</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E47" s="32" t="s">
         <v>22</v>
@@ -13732,13 +13732,13 @@
         <v>29.555</v>
       </c>
       <c r="H47" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="I47" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="J47" s="53" t="s">
         <v>190</v>
-      </c>
-      <c r="I47" s="55" t="s">
-        <v>190</v>
-      </c>
-      <c r="J47" s="53" t="s">
-        <v>191</v>
       </c>
       <c r="K47" s="37">
         <v>-92.305000000000007</v>
@@ -13769,10 +13769,10 @@
         <v>8768094</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E48" s="32" t="s">
         <v>22</v>
@@ -13822,10 +13822,10 @@
         <v>8770822</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E49" s="32" t="s">
         <v>22</v>
@@ -13837,13 +13837,13 @@
         <v>29.688330000000001</v>
       </c>
       <c r="H49" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="I49" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="J49" s="54" t="s">
         <v>190</v>
-      </c>
-      <c r="I49" s="55" t="s">
-        <v>190</v>
-      </c>
-      <c r="J49" s="54" t="s">
-        <v>191</v>
       </c>
       <c r="K49" s="48">
         <v>-93.839780000000005</v>
@@ -13874,10 +13874,10 @@
         <v>8772471</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E50" s="32" t="s">
         <v>22</v>
@@ -13889,13 +13889,13 @@
         <v>28.934999999999999</v>
       </c>
       <c r="H50" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="I50" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="J50" s="53" t="s">
         <v>190</v>
-      </c>
-      <c r="I50" s="55" t="s">
-        <v>190</v>
-      </c>
-      <c r="J50" s="53" t="s">
-        <v>191</v>
       </c>
       <c r="K50" s="37">
         <v>-95.295000000000002</v>
@@ -13926,10 +13926,10 @@
         <v>8773767</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E51" s="32" t="s">
         <v>22</v>
@@ -13948,7 +13948,7 @@
         <v>-8.9911612313319095E-2</v>
       </c>
       <c r="J51" s="53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K51" s="37">
         <v>-96.330100000000002</v>
@@ -13979,10 +13979,10 @@
         <v>8775241</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E52" s="32" t="s">
         <v>22</v>
@@ -13994,13 +13994,13 @@
         <v>27.836670000000002</v>
       </c>
       <c r="H52" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="I52" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="J52" s="53" t="s">
         <v>190</v>
-      </c>
-      <c r="I52" s="55" t="s">
-        <v>190</v>
-      </c>
-      <c r="J52" s="53" t="s">
-        <v>191</v>
       </c>
       <c r="K52" s="37">
         <v>-97.038330000000002</v>
@@ -14031,10 +14031,10 @@
         <v>8775870</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E53" s="32" t="s">
         <v>22</v>
@@ -14084,10 +14084,10 @@
         <v>8779748</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E54" s="32" t="s">
         <v>22</v>
@@ -14285,10 +14285,10 @@
     <row r="62" spans="1:28" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="59"/>
       <c r="B62" s="60" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" s="91" t="s">
         <v>197</v>
-      </c>
-      <c r="C62" s="91" t="s">
-        <v>198</v>
       </c>
       <c r="D62" s="92"/>
       <c r="E62" s="92"/>
@@ -44101,7 +44101,7 @@
         <v>8747437</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>144</v>
@@ -44142,10 +44142,10 @@
         <v>8760922</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>22</v>
@@ -44183,10 +44183,10 @@
         <v>8761305</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>22</v>
@@ -44224,10 +44224,10 @@
         <v>8761724</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>22</v>
@@ -44265,10 +44265,10 @@
         <v>8764314</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>22</v>
@@ -44306,10 +44306,10 @@
         <v>8766072</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>22</v>
@@ -44321,10 +44321,10 @@
         <v>29.555</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J47" s="11">
         <v>-92.305000000000007</v>
@@ -44346,10 +44346,10 @@
         <v>8768094</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>22</v>
@@ -44387,10 +44387,10 @@
         <v>8770822</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>22</v>
@@ -44402,10 +44402,10 @@
         <v>29.688330000000001</v>
       </c>
       <c r="H49" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J49" s="18">
         <v>-93.839780000000005</v>
@@ -44427,10 +44427,10 @@
         <v>8772471</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>22</v>
@@ -44442,10 +44442,10 @@
         <v>28.934999999999999</v>
       </c>
       <c r="H50" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J50" s="11">
         <v>-95.295000000000002</v>
@@ -44467,10 +44467,10 @@
         <v>8773767</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>22</v>
@@ -44508,10 +44508,10 @@
         <v>8775241</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>22</v>
@@ -44523,10 +44523,10 @@
         <v>27.836670000000002</v>
       </c>
       <c r="H52" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J52" s="11">
         <v>-97.038330000000002</v>
@@ -44548,10 +44548,10 @@
         <v>8775870</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>22</v>
@@ -44589,10 +44589,10 @@
         <v>8779748</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>22</v>

</xml_diff>